<commit_message>
Add videos and PDF
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisa/Desktop/RSIG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD46E52-9E57-1E47-B32F-47569FBB4B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9999EA2-AE28-2249-BE97-9B2E8E77A0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>First Author Province</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Co Authors</t>
   </si>
   <si>
     <t>Abstract File Type</t>
@@ -288,9 +282,6 @@
     <t>Submitting What</t>
   </si>
   <si>
-    <t>TITLE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Evaluating the Role of Strengths in Positive Outcomes for Justice-Involved Youth With FASD: A Scoping Review </t>
   </si>
   <si>
@@ -304,9 +295,6 @@
   </si>
   <si>
     <t>Compatibility of Roommates on the Autism Spectrum: A Scoping Review</t>
-  </si>
-  <si>
-    <t>Contact Author</t>
   </si>
   <si>
     <t>Meghan McMurtry, University of Guelph,
@@ -315,12 +303,6 @@
 Kaitlyn McLachlan, University of Guelph, CanFASD</t>
   </si>
   <si>
-    <t>Video File</t>
-  </si>
-  <si>
-    <t>PDF File</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -366,24 +348,6 @@
     <t>https://youtu.be/HZkhGNwRGcA</t>
   </si>
   <si>
-    <t>https://docs.google.com/presentation/d/1alArig6KFzh89VDK1JekU3dGGxzsQ9br/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1640aBO7Nk0hwUN9q57BKsc_YusSWR0In/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1EeTw9mOyR4D1gd79BJ-UsVPPT3U00dXK/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/presentation/d/1855yp6nG2jUf1cTbz7CBgLTCQkDXYPfv/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1H3tCgteKPqg4z0D_Mwl14ZGo8gOP9-4L/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>Embedded Link</t>
-  </si>
-  <si>
     <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/7WuckrjCfa8" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
   </si>
   <si>
@@ -426,9 +390,6 @@
     <t>virginie.cobigo@uOttawa.ca</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1EUFdAq5lri__WLO1WBWXahZECFuWl4CW/view?usp=sharing</t>
-  </si>
-  <si>
     <t>Powerpoints</t>
   </si>
   <si>
@@ -447,12 +408,6 @@
     <t>odobson@uoguelph.ca</t>
   </si>
   <si>
-    <t>https://docs.google.com/presentation/d/1xtSsJwOhu9fA-KVzoS92WS78-q10h_VO/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/document/d/1cc9TiSJM-uVXGp6chmdI6HlbcvrrwwRz/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
     <t>Exploring a Good Life with People with an Intellectual Disability Using Participatory Audio/Visual Methods</t>
   </si>
   <si>
@@ -462,12 +417,6 @@
     <t>josee.boulanger@uottawa.ca</t>
   </si>
   <si>
-    <t>https://docs.google.com/presentation/d/1OnwO08g1UO4EHrPqY6I-2VmPtyYjTeha/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/document/d/10lE9L7gvZtdwYhHDa11PALFRvEjJTnvh/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -483,9 +432,6 @@
     <t>star7980@mylaurier.ca</t>
   </si>
   <si>
-    <t>https://docs.google.com/presentation/d/1lAttFYWa3zgLbE2ooBAxFm0348sq8DmV/edit?usp=sharing&amp;ouid=113063826871228842098&amp;rtpof=true&amp;sd=true</t>
-  </si>
-  <si>
     <t>Program</t>
   </si>
   <si>
@@ -504,9 +450,6 @@
     <t>https://forms.gle/mUDznH86rUYiAPtv9</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1Zm3vzXcdEBW_p74XR1eOzWbWEguGNV6m/view?usp=sharing</t>
-  </si>
-  <si>
     <t>COVID-19 Pandemic: Parents Find Innovative Ways to Connect with Their Children Who Reside in Supported Independent Living Environments</t>
   </si>
   <si>
@@ -516,7 +459,67 @@
     <t>penrose1@uwindsor.ca</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1E6lFsKYaKk4zPJ2Q6duTPboWwjzPqa2h/view?usp=sharing</t>
+    <t>ANDREASEN.PDF</t>
+  </si>
+  <si>
+    <t>Babikian.pdf</t>
+  </si>
+  <si>
+    <t>Bibr.pdf</t>
+  </si>
+  <si>
+    <t>Boulanger_Script.docx</t>
+  </si>
+  <si>
+    <t>Boulanger_Slides.pptx</t>
+  </si>
+  <si>
+    <t>Bumbacco.pdf</t>
+  </si>
+  <si>
+    <t>Cobigo_Slides.pdf</t>
+  </si>
+  <si>
+    <t>Dobson_Script.docx</t>
+  </si>
+  <si>
+    <t>Dobson_Slides.pptx</t>
+  </si>
+  <si>
+    <t>Formuli.pdf</t>
+  </si>
+  <si>
+    <t>Kozluk.pptx</t>
+  </si>
+  <si>
+    <t>Penrose_slides.pdf</t>
+  </si>
+  <si>
+    <t>Vanwyck &amp; Halar_Slides.pptx</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>contactAuthor</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>coAuthors</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>embed</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -593,13 +596,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -768,9 +764,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -783,6 +776,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1122,733 +1116,779 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91ED4234-2111-054E-91AA-E7AB4F3EFD0B}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="45"/>
-    <col min="2" max="2" width="100" style="45" customWidth="1"/>
-    <col min="3" max="3" width="17" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.33203125" style="45" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.83203125" style="45" customWidth="1"/>
-    <col min="10" max="13" width="0" style="45" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="43.1640625" style="45" customWidth="1"/>
-    <col min="16" max="19" width="10.83203125" style="45"/>
+    <col min="1" max="2" width="10.83203125" style="45"/>
+    <col min="3" max="3" width="100" style="45" customWidth="1"/>
+    <col min="4" max="4" width="17" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="10.33203125" style="45" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="84.83203125" style="45" customWidth="1"/>
+    <col min="11" max="14" width="0" style="45" hidden="1" customWidth="1"/>
+    <col min="15" max="16" width="43.1640625" style="45" customWidth="1"/>
+    <col min="17" max="20" width="10.83203125" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>82</v>
+        <v>152</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="N1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>84</v>
-      </c>
       <c r="O1" s="19" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="P1" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q1" s="19"/>
+        <v>150</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>151</v>
+      </c>
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
-    </row>
-    <row r="2" spans="1:19" s="18" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="T1" s="19"/>
+    </row>
+    <row r="2" spans="1:20" s="18" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B2" s="22">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
-    </row>
-    <row r="3" spans="1:19" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="T2" s="22"/>
+    </row>
+    <row r="3" spans="1:20" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="36">
+        <v>2</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="48" t="s">
+        <v>16</v>
+      </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
-      <c r="H3" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>12</v>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>40</v>
       </c>
       <c r="K3" s="48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="51"/>
-      <c r="O3" s="36"/>
+        <v>9</v>
+      </c>
+      <c r="M3" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="51"/>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
       <c r="R3" s="36"/>
       <c r="S3" s="36"/>
-    </row>
-    <row r="4" spans="1:19" s="16" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T3" s="36"/>
+    </row>
+    <row r="4" spans="1:20" s="16" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="30"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="28">
+        <v>3</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="H4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>12</v>
+      <c r="H4" s="30"/>
+      <c r="I4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="K4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q4" s="28"/>
+      <c r="N4" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28" t="s">
+        <v>96</v>
+      </c>
       <c r="R4" s="28"/>
       <c r="S4" s="28"/>
-    </row>
-    <row r="5" spans="1:19" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="T4" s="28"/>
+    </row>
+    <row r="5" spans="1:20" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="30"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="28">
+        <v>4</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
-      <c r="H5" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="29" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>104</v>
+      <c r="O5" s="46" t="s">
+        <v>85</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q5" s="28"/>
+        <v>134</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>97</v>
+      </c>
       <c r="R5" s="28"/>
       <c r="S5" s="28"/>
-    </row>
-    <row r="6" spans="1:19" s="16" customFormat="1" ht="189" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T5" s="28"/>
+    </row>
+    <row r="6" spans="1:20" s="16" customFormat="1" ht="189" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="30"/>
+        <v>12</v>
+      </c>
+      <c r="B6" s="28">
+        <v>5</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>12</v>
+      <c r="H6" s="30"/>
+      <c r="I6" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="K6" s="30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="O6" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="P6" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q6" s="28"/>
+        <v>11</v>
+      </c>
+      <c r="M6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="P6" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="R6" s="28"/>
       <c r="S6" s="28"/>
-    </row>
-    <row r="7" spans="1:19" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="T6" s="28"/>
+    </row>
+    <row r="7" spans="1:20" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="B7" s="22">
+        <v>6</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="24"/>
+      <c r="I7" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="24" t="s">
+      <c r="L7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="O7" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q7" s="22"/>
+      <c r="N7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>100</v>
+      </c>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
-    </row>
-    <row r="8" spans="1:19" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="T7" s="22"/>
+    </row>
+    <row r="8" spans="1:20" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="38"/>
+        <v>12</v>
+      </c>
+      <c r="B8" s="36">
+        <v>7</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>45</v>
+      </c>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
-      <c r="H8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38" t="s">
-        <v>12</v>
-      </c>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="38"/>
       <c r="K8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="36"/>
+      <c r="N8" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
       <c r="R8" s="36"/>
       <c r="S8" s="36"/>
-    </row>
-    <row r="9" spans="1:19" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="T8" s="36"/>
+    </row>
+    <row r="9" spans="1:20" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="33"/>
+        <v>12</v>
+      </c>
+      <c r="B9" s="28">
+        <v>8</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>52</v>
+      </c>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
-      <c r="H9" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="32" t="s">
+      <c r="H9" s="33"/>
+      <c r="I9" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="28" t="s">
-        <v>94</v>
-      </c>
       <c r="O9" s="28" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q9" s="28"/>
+        <v>133</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>101</v>
+      </c>
       <c r="R9" s="28"/>
       <c r="S9" s="28"/>
-    </row>
-    <row r="10" spans="1:19" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="T9" s="28"/>
+    </row>
+    <row r="10" spans="1:20" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="42"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="22">
+        <v>9</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>57</v>
+      </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
-      <c r="H10" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="42" t="s">
+      <c r="H10" s="42"/>
+      <c r="I10" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="N10" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q10" s="22"/>
+      <c r="O10" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
+        <v>99</v>
+      </c>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
-    </row>
-    <row r="11" spans="1:19" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="T10" s="22"/>
+    </row>
+    <row r="11" spans="1:20" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="42"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="22">
+        <v>10</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>65</v>
+      </c>
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
-      <c r="H11" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>69</v>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="K11" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q11" s="22"/>
+      <c r="N11" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22" t="s">
+        <v>98</v>
+      </c>
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
-    </row>
-    <row r="12" spans="1:19" s="16" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="T11" s="22"/>
+    </row>
+    <row r="12" spans="1:20" s="16" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="33"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="28">
+        <v>11</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>69</v>
+      </c>
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="33"/>
+      <c r="I12" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="O12" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="P12" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q12" s="28"/>
+      <c r="O12" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="P12" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q12" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
-    </row>
-    <row r="13" spans="1:19" s="16" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T12" s="28"/>
+    </row>
+    <row r="13" spans="1:20" s="16" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28">
+        <v>12</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
-      <c r="H13" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="30" t="s">
-        <v>12</v>
+      <c r="H13" s="30"/>
+      <c r="I13" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="K13" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="R13" s="28"/>
       <c r="S13" s="28"/>
-    </row>
-    <row r="14" spans="1:19" s="16" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T13" s="28"/>
+    </row>
+    <row r="14" spans="1:20" s="16" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="28">
+        <v>13</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
-      <c r="H14" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>12</v>
+      <c r="H14" s="30"/>
+      <c r="I14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>43</v>
       </c>
       <c r="K14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="O14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28" t="s">
+        <v>92</v>
+      </c>
       <c r="P14" s="28"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
       <c r="S14" s="28"/>
-    </row>
-    <row r="15" spans="1:19" s="16" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T14" s="28"/>
+    </row>
+    <row r="15" spans="1:20" s="16" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="33"/>
+      <c r="C15" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="G15" s="33"/>
-      <c r="H15" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="33" t="s">
-        <v>52</v>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28" t="s">
-        <v>99</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="M15" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="28"/>
       <c r="O15" s="28" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="P15" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q15" s="28"/>
+        <v>142</v>
+      </c>
+      <c r="Q15" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
-    </row>
-    <row r="16" spans="1:19" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T15" s="28"/>
+    </row>
+    <row r="16" spans="1:20" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="38"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="36">
+        <v>15</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>62</v>
+      </c>
       <c r="E16" s="38"/>
       <c r="F16" s="38"/>
       <c r="G16" s="38"/>
-      <c r="H16" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="38" t="s">
-        <v>66</v>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39" t="s">
+        <v>63</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="K16" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="M16" s="36"/>
       <c r="N16" s="36"/>
       <c r="O16" s="36"/>
       <c r="P16" s="36"/>
       <c r="Q16" s="36"/>
       <c r="R16" s="36"/>
       <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{B8B5738C-E38E-1941-9251-9092A5080C31}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{29D16A6A-B90B-F645-940A-DF69E4701E2A}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{AAB23955-FB00-D245-AC7B-8B9B84F38E8C}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{BA6B7616-1691-4746-BC51-C27F98381AA6}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{6689E25E-70BB-3C48-A1E3-6D354612A3B6}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{CCF5F949-6E30-244F-AB01-2A9C99DF8B6E}"/>
-    <hyperlink ref="H13" r:id="rId7" xr:uid="{C83CD9C0-399D-4246-839A-5048B980DC46}"/>
-    <hyperlink ref="H14" r:id="rId8" xr:uid="{A696B89A-61B6-8B41-A1E5-A3462C09F319}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{9A7475F1-7DCE-234A-B4F2-0F02D8900C09}"/>
-    <hyperlink ref="H11" r:id="rId10" xr:uid="{840B02D3-1572-6346-A3C7-F6F179695250}"/>
-    <hyperlink ref="H12" r:id="rId11" xr:uid="{0470869B-8642-E74C-BA29-4D4DBCB1177D}"/>
-    <hyperlink ref="H15" r:id="rId12" xr:uid="{3A5FD724-3778-8943-9C5A-DDEAAB5E4900}"/>
-    <hyperlink ref="H16" r:id="rId13" xr:uid="{A0EB3DAF-FE2E-9A4C-9B01-B8C93F6C92FB}"/>
-    <hyperlink ref="H9" r:id="rId14" xr:uid="{1A4D673C-2FB1-644C-B88E-4CBC0F38B3EA}"/>
-    <hyperlink ref="N2" r:id="rId15" xr:uid="{7DC64451-BAD4-EF40-8268-D167821EC117}"/>
-    <hyperlink ref="N4" r:id="rId16" xr:uid="{54E4972A-6D95-3A4E-8FE9-BB5D703DF06E}"/>
-    <hyperlink ref="N5" r:id="rId17" xr:uid="{1F5EFB46-F0F8-0D45-BFF3-18BAC9D1C583}"/>
-    <hyperlink ref="N7" r:id="rId18" xr:uid="{509190F4-DA03-1742-9FD1-16B66F5B1853}"/>
-    <hyperlink ref="O6" r:id="rId19" xr:uid="{27654A50-4195-7446-9F81-070038841592}"/>
-    <hyperlink ref="O12" r:id="rId20" xr:uid="{CED6A682-A14E-DC46-BFA4-143FD9A8B512}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{B8B5738C-E38E-1941-9251-9092A5080C31}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{29D16A6A-B90B-F645-940A-DF69E4701E2A}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{AAB23955-FB00-D245-AC7B-8B9B84F38E8C}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{BA6B7616-1691-4746-BC51-C27F98381AA6}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{6689E25E-70BB-3C48-A1E3-6D354612A3B6}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{CCF5F949-6E30-244F-AB01-2A9C99DF8B6E}"/>
+    <hyperlink ref="I13" r:id="rId7" xr:uid="{C83CD9C0-399D-4246-839A-5048B980DC46}"/>
+    <hyperlink ref="I14" r:id="rId8" xr:uid="{A696B89A-61B6-8B41-A1E5-A3462C09F319}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{9A7475F1-7DCE-234A-B4F2-0F02D8900C09}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{840B02D3-1572-6346-A3C7-F6F179695250}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{0470869B-8642-E74C-BA29-4D4DBCB1177D}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{3A5FD724-3778-8943-9C5A-DDEAAB5E4900}"/>
+    <hyperlink ref="I16" r:id="rId13" xr:uid="{A0EB3DAF-FE2E-9A4C-9B01-B8C93F6C92FB}"/>
+    <hyperlink ref="I9" r:id="rId14" xr:uid="{1A4D673C-2FB1-644C-B88E-4CBC0F38B3EA}"/>
+    <hyperlink ref="O2" r:id="rId15" xr:uid="{7DC64451-BAD4-EF40-8268-D167821EC117}"/>
+    <hyperlink ref="O4" r:id="rId16" xr:uid="{54E4972A-6D95-3A4E-8FE9-BB5D703DF06E}"/>
+    <hyperlink ref="O5" r:id="rId17" xr:uid="{1F5EFB46-F0F8-0D45-BFF3-18BAC9D1C583}"/>
+    <hyperlink ref="O7" r:id="rId18" xr:uid="{509190F4-DA03-1742-9FD1-16B66F5B1853}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1862,7 +1902,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1901,19 +1941,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -1941,16 +1981,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>121</v>
+        <v>108</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>138</v>
       </c>
       <c r="F2" s="57"/>
       <c r="I2" s="4"/>
@@ -1977,19 +2017,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>125</v>
+        <v>111</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>112</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>129</v>
+        <v>114</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>139</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -2011,23 +2051,23 @@
       <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="61">
+      <c r="A4" s="60">
         <v>3</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>134</v>
+        <v>115</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>135</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -2049,22 +2089,22 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="62" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="63" t="s">
-        <v>148</v>
+      <c r="A5" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>129</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="63"/>
+        <v>131</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="62"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -2087,22 +2127,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="62" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="63"/>
+      <c r="A6" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="62"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2682,32 +2722,32 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="52" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="52" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>